<commit_message>
exercise 2 from page 51 - solution
</commit_message>
<xml_diff>
--- a/year 1 sem 2 ПИ/u3/otched3.xlsx
+++ b/year 1 sem 2 ПИ/u3/otched3.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\apps\programming\tu-sofia\year 1 sem 2 ПИ\u3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C341B5-2C0E-4768-82EB-9C955208E8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4410" yWindow="1230" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,130 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+  <si>
+    <t>Пореден Номер</t>
+  </si>
+  <si>
+    <t>Описание</t>
+  </si>
+  <si>
+    <t>Връзка</t>
+  </si>
+  <si>
+    <t>Време</t>
+  </si>
+  <si>
+    <t>16:45 - 17:00</t>
+  </si>
+  <si>
+    <t>17:00 - 17:15</t>
+  </si>
+  <si>
+    <t>17:15 - 17:30</t>
+  </si>
+  <si>
+    <t>17:45 - 18:30</t>
+  </si>
+  <si>
+    <t>18:45 - 19:00</t>
+  </si>
+  <si>
+    <t>Пример1_21</t>
+  </si>
+  <si>
+    <t>Пример2_21</t>
+  </si>
+  <si>
+    <t>Пример3_22</t>
+  </si>
+  <si>
+    <t>Задача1_22</t>
+  </si>
+  <si>
+    <t>Задача2_22</t>
+  </si>
+  <si>
+    <t>Задача3_22</t>
+  </si>
+  <si>
+    <t>19:00 - 19:30</t>
+  </si>
+  <si>
+    <t>p1_21.c</t>
+  </si>
+  <si>
+    <t>p2_21.c</t>
+  </si>
+  <si>
+    <t>p3_22.c</t>
+  </si>
+  <si>
+    <t>z1_22.c</t>
+  </si>
+  <si>
+    <t>z2_22.c</t>
+  </si>
+  <si>
+    <t>z3_22.c</t>
+  </si>
+  <si>
+    <t>Сумиране на две числа</t>
+  </si>
+  <si>
+    <t>Въвеждане и извеждане на възраст на потребителя</t>
+  </si>
+  <si>
+    <t>От Целзий в Фаренхайт</t>
+  </si>
+  <si>
+    <t>Отпечатване на трите имена и факултетен номер</t>
+  </si>
+  <si>
+    <t xml:space="preserve">самолет - мили в километри </t>
+  </si>
+  <si>
+    <t>решаване на математическа задача по дадена формула</t>
+  </si>
+  <si>
+    <t>Име:</t>
+  </si>
+  <si>
+    <t>Виктор Мирославов Методиев</t>
+  </si>
+  <si>
+    <t>Задачи</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,13 +172,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +471,160 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="70.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="D8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{FA01E1F2-DB51-4BA4-91D5-53D1724DA108}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{687A34CF-3F68-416E-A836-E51DA1149A1D}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{A4913E28-0E9C-4231-AD2C-23587CD3BA5C}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{9F1145CB-8773-4214-8D45-612905BE75F1}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{B66F1DC4-DDC6-4B5D-BAD4-E388B0761202}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{B1BC8E04-ECFE-4FEB-841A-A15662C6E5DD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>